<commit_message>
Fixed bug cog shift factor rigging
</commit_message>
<xml_diff>
--- a/app/Data_input/Constants_DNV.xlsx
+++ b/app/Data_input/Constants_DNV.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Viktor_apps\Rigging_app\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Viktor_apps_good\Rigging_App\app\Data_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373968D7-4E75-457B-9425-362272A4F75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EC293A-DAF1-45C9-99F5-A974C8636191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B2781BCC-0105-49AB-92BD-AA2FC97DD61D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{B2781BCC-0105-49AB-92BD-AA2FC97DD61D}"/>
   </bookViews>
   <sheets>
     <sheet name="COGCrane" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="57">
   <si>
     <t>Multihook on single vessel</t>
   </si>
@@ -181,9 +181,6 @@
   </si>
   <si>
     <t xml:space="preserve">Values </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use of COG envelope </t>
   </si>
   <si>
     <t>Standard COG envlope</t>
@@ -944,7 +941,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -952,7 +949,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>1.25</v>
@@ -960,7 +957,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4">
         <v>1.1000000000000001</v>
@@ -968,7 +965,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -983,7 +980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD198AFE-D826-4BA5-9926-E8E171FF2EA2}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1002,44 +999,44 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" s="13"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="13"/>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>54</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>55</v>
       </c>
       <c r="C6" s="22"/>
     </row>
@@ -1052,8 +1049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE428A19-CE40-4906-97BB-1F63D1E9BCAA}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1071,15 +1068,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>1.1000000000000001</v>

</xml_diff>